<commit_message>
scripts feitos (ddl,dml,dql feitos)
</commit_message>
<xml_diff>
--- a/Exercicios/1.3-exercicio-pclinics/Modelagem/1.3-exercicio-pclinics-fisico.xlsx
+++ b/Exercicios/1.3-exercicio-pclinics/Modelagem/1.3-exercicio-pclinics-fisico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55119\Desktop\Trabalhos Nayara 2021\SENAI\2º Semestre\Exercicios\1.3-exercicio-pclinics\Modelagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{906D9CCC-76D9-46BB-9E05-7E21D4B58824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85AFB94-E78F-486D-AD77-3317A6257EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1277C621-C1C3-462A-8198-0BE85094CE13}"/>
+    <workbookView xWindow="6585" yWindow="1815" windowWidth="13260" windowHeight="7875" xr2:uid="{1277C621-C1C3-462A-8198-0BE85094CE13}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -170,9 +170,6 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -192,6 +189,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -511,217 +511,220 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K9"/>
+      <selection activeCell="B2" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="1" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="7" t="s">
+      <c r="I2" s="1"/>
+      <c r="J2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="5">
-        <v>1</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="D3" s="1"/>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>2</v>
       </c>
-      <c r="H3" s="7">
-        <v>1</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="7">
-        <v>1</v>
-      </c>
-      <c r="K3" s="4" t="s">
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="6">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="5">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="4">
         <v>2</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="6">
-        <v>1</v>
-      </c>
-      <c r="H4" s="7">
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6">
         <v>2</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="7">
+      <c r="I4" s="1"/>
+      <c r="J4" s="6">
         <v>2</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="1" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="2"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="1"/>
+      <c r="E7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="2"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>1</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="5">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="3">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6">
-        <v>1</v>
-      </c>
-      <c r="H8" s="8">
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7">
         <v>44432</v>
       </c>
-      <c r="I8" s="2"/>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>2</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="3">
-        <v>1</v>
-      </c>
-      <c r="F9" s="5">
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4">
         <v>2</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>2</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <v>44433</v>
       </c>
-      <c r="I9" s="2"/>
+      <c r="I9" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>